<commit_message>
Reran DAVID after removing the T051 outlier sample
</commit_message>
<xml_diff>
--- a/output/Func_annot_DAVID/FOA_BP_DAVID.xlsx
+++ b/output/Func_annot_DAVID/FOA_BP_DAVID.xlsx
@@ -1,69 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8DA1D38-1F87-C642-A137-642345DC3AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26C62931-7841-B745-86EE-9696BF313319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{10D8521F-3C48-D340-9DC3-7FC8878A2082}"/>
+    <workbookView xWindow="680" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6F1DE110-3671-B248-AD29-147BAFE6905D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FOA_BP_DAVID" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="FOA_BP_DAVID" localSheetId="0">Sheet1!$A$1:$M$23</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{4B77C044-0F4F-8E49-9C47-B9A2EFB3E8AF}" name="FOA_BP_DAVID" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/graceleuchtenberger/Desktop/FOA_BP_DAVID">
-      <textFields count="13">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>Category</t>
   </si>
@@ -101,7 +58,7 @@
     <t>Benjamini</t>
   </si>
   <si>
-    <t>FDR</t>
+    <t>FDR\</t>
   </si>
   <si>
     <t>GOTERM_BP_DIRECT</t>
@@ -110,7 +67,10 @@
     <t>GO:0006418~tRNA aminoacylation for protein translation</t>
   </si>
   <si>
-    <t>Q9P2J5, P41250, Q99MN1, P49588, Q9D0R2</t>
+    <t>Q9P2J5, P41250, P49588, Q6PF21</t>
+  </si>
+  <si>
+    <t>0.006342774087812532\</t>
   </si>
   <si>
     <t>GO:0006413~translational initiation</t>
@@ -119,34 +79,52 @@
     <t>Q7SXU0, O60841, O43432, Q99L45, F1QGW6, P59325</t>
   </si>
   <si>
-    <t>GO:0006412~translation</t>
-  </si>
-  <si>
-    <t>Q7SXU0, Q99MN1, Q99L45, F1QGW6, P59325, Q1JPX3, Q6PF21, Q9D0R2</t>
-  </si>
-  <si>
     <t>GO:0001731~formation of translation preinitiation complex</t>
   </si>
   <si>
     <t>Q99L45, F1QGW6, P59325</t>
   </si>
   <si>
+    <t>0.23966545224291821\</t>
+  </si>
+  <si>
     <t>GO:0006446~regulation of translational initiation</t>
   </si>
   <si>
     <t>O60841, O43432, P59325</t>
   </si>
   <si>
+    <t>0.5465453046494814\</t>
+  </si>
+  <si>
     <t>GO:0001732~formation of cytoplasmic translation initiation complex</t>
   </si>
   <si>
     <t>Q7SXU0, Q99L45, P59325</t>
   </si>
   <si>
-    <t>GO:0051085~chaperone cofactor-dependent protein refolding</t>
-  </si>
-  <si>
-    <t>Q5DC69, Q5ZM98, Q5ZL72</t>
+    <t>0.6819722544749924\</t>
+  </si>
+  <si>
+    <t>GO:0015966~diadenosine tetraphosphate biosynthetic process</t>
+  </si>
+  <si>
+    <t>P41250, Q99MN1</t>
+  </si>
+  <si>
+    <t>1.0\</t>
+  </si>
+  <si>
+    <t>GO:0070327~thyroid hormone transport</t>
+  </si>
+  <si>
+    <t>Q5RAE3, Q01650</t>
+  </si>
+  <si>
+    <t>GO:0014850~response to muscle activity</t>
+  </si>
+  <si>
+    <t>P28650, Q01650</t>
   </si>
   <si>
     <t>GO:0043032~positive regulation of macrophage activation</t>
@@ -155,36 +133,6 @@
     <t>Q99MN1, Q5ZL72</t>
   </si>
   <si>
-    <t>GO:0015966~diadenosine tetraphosphate biosynthetic process</t>
-  </si>
-  <si>
-    <t>P41250, Q99MN1</t>
-  </si>
-  <si>
-    <t>GO:0014850~response to muscle activity</t>
-  </si>
-  <si>
-    <t>P28650, Q01650</t>
-  </si>
-  <si>
-    <t>GO:0001514~selenocysteine incorporation</t>
-  </si>
-  <si>
-    <t>P26636, F1QGW6</t>
-  </si>
-  <si>
-    <t>GO:0070327~thyroid hormone transport</t>
-  </si>
-  <si>
-    <t>Q5RAE3, Q01650</t>
-  </si>
-  <si>
-    <t>GO:0043039~tRNA aminoacylation</t>
-  </si>
-  <si>
-    <t>Q1JPX3, Q9D0R2</t>
-  </si>
-  <si>
     <t>GO:0106074~aminoacyl-tRNA metabolism involved in translational fidelity</t>
   </si>
   <si>
@@ -197,47 +145,68 @@
     <t>O60841, P59325</t>
   </si>
   <si>
+    <t>GO:0032729~positive regulation of type II interferon production</t>
+  </si>
+  <si>
+    <t>Q01650, Q5ZL72</t>
+  </si>
+  <si>
+    <t>GO:0034260~negative regulation of GTPase activity</t>
+  </si>
+  <si>
+    <t>Q9JIH7, Q14684</t>
+  </si>
+  <si>
     <t>GO:0042026~protein refolding</t>
   </si>
   <si>
     <t>Q5ZM98, Q5ZL72</t>
   </si>
   <si>
-    <t>GO:0032729~positive regulation of type II interferon production</t>
-  </si>
-  <si>
-    <t>Q01650, Q5ZL72</t>
+    <t>GO:0003333~amino acid transmembrane transport</t>
+  </si>
+  <si>
+    <t>GO:0006541~glutamine metabolic process</t>
+  </si>
+  <si>
+    <t>P28650, Q5ZJU3</t>
   </si>
   <si>
     <t>GO:0015804~neutral amino acid transport</t>
   </si>
   <si>
+    <t>GO:0042274~ribosomal small subunit biogenesis</t>
+  </si>
+  <si>
+    <t>Q6AXX4, O00567, O00566</t>
+  </si>
+  <si>
     <t>GO:0006400~tRNA modification</t>
   </si>
   <si>
     <t>P26636, P49588</t>
   </si>
   <si>
-    <t>GO:0003333~amino acid transmembrane transport</t>
-  </si>
-  <si>
-    <t>GO:0006541~glutamine metabolic process</t>
-  </si>
-  <si>
-    <t>P28650, Q5ZJU3</t>
-  </si>
-  <si>
-    <t>GO:0042274~ribosomal small subunit biogenesis</t>
-  </si>
-  <si>
-    <t>Q6AXX4, O00567, O00566</t>
+    <t>GO:0042113~B cell activation</t>
+  </si>
+  <si>
+    <t>Q5RAE3, Q5XIH7</t>
+  </si>
+  <si>
+    <t>GO:0002183~cytoplasmic translational initiation</t>
+  </si>
+  <si>
+    <t>Q99L45, F1QGW6</t>
+  </si>
+  <si>
+    <t>1.0}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -245,16 +214,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -262,16 +531,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -284,10 +742,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FOA_BP_DAVID" connectionId="1" xr16:uid="{A2D29462-6438-1743-BB69-2B0CBC39EAB2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -606,23 +1060,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317F5941-3A0B-6D43-8102-DEBC97D5EBBB}">
-  <dimension ref="A1:M23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AB07A9-6E2C-1444-9089-A66C64CD7585}">
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -674,37 +1122,37 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>8.3333333333333304</v>
+        <v>6.6666666666666599</v>
       </c>
       <c r="E2" s="1">
-        <v>1.41699920750998E-6</v>
+        <v>3.53718172052578E-5</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="G2">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I2">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J2">
-        <v>50.989898989898897</v>
-      </c>
-      <c r="K2" s="1">
-        <v>4.7741507240528502E-4</v>
-      </c>
-      <c r="L2" s="1">
-        <v>4.7752873293086402E-4</v>
-      </c>
-      <c r="M2" s="1">
-        <v>4.7611173372335397E-4</v>
+        <v>54.264150943396203</v>
+      </c>
+      <c r="K2">
+        <v>1.1884698052375501E-2</v>
+      </c>
+      <c r="L2">
+        <v>6.3427740878125296E-3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -712,7 +1160,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -721,31 +1169,31 @@
         <v>10</v>
       </c>
       <c r="E3" s="1">
-        <v>5.0676481547797298E-5</v>
+        <v>3.7531207620192499E-5</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H3">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J3">
-        <v>14.120279720279701</v>
+        <v>14.9940417080436</v>
       </c>
       <c r="K3">
-        <v>1.69333977117056E-2</v>
+        <v>1.2605660823186499E-2</v>
       </c>
       <c r="L3">
-        <v>8.5389871408038404E-3</v>
-      </c>
-      <c r="M3">
-        <v>8.5136489000299399E-3</v>
+        <v>6.3427740878125296E-3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -753,40 +1201,40 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>13.3333333333333</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3.4110993813996499E-4</v>
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>2.12720815600223E-3</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H4">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="I4">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J4">
-        <v>5.8274170274170203</v>
+        <v>40.698113207547102</v>
       </c>
       <c r="K4">
-        <v>0.108610376840613</v>
+        <v>0.51313196618274304</v>
       </c>
       <c r="L4">
-        <v>3.8318016384389399E-2</v>
-      </c>
-      <c r="M4">
-        <v>3.8204313071676099E-2</v>
+        <v>0.23966545224291799</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -794,7 +1242,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -803,31 +1251,31 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>1.6392506144592099E-3</v>
+        <v>6.4679917709997798E-3</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G5">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I5">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J5">
-        <v>45.890909090908998</v>
+        <v>23.7405660377358</v>
       </c>
       <c r="K5">
-        <v>0.42470983806960899</v>
+        <v>0.88844995498456403</v>
       </c>
       <c r="L5">
-        <v>0.13810686426818899</v>
-      </c>
-      <c r="M5">
-        <v>0.13769705161457399</v>
+        <v>0.54654530464948103</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -835,7 +1283,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -844,31 +1292,31 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>6.9217971738657104E-3</v>
+        <v>1.0088346959689199E-2</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G6">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J6">
-        <v>22.945454545454499</v>
+        <v>18.992452830188601</v>
       </c>
       <c r="K6">
-        <v>0.90374517194228998</v>
+        <v>0.96752152659306601</v>
       </c>
       <c r="L6">
-        <v>0.46652912951854902</v>
-      </c>
-      <c r="M6">
-        <v>0.46514477008377503</v>
+        <v>0.68197225447499199</v>
+      </c>
+      <c r="M6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -876,40 +1324,40 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>3.3333333333333299</v>
       </c>
       <c r="E7">
-        <v>1.0788331447860599E-2</v>
+        <v>2.05589058159583E-2</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G7">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H7">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J7">
-        <v>18.3563636363636</v>
+        <v>94.962264150943398</v>
       </c>
       <c r="K7">
-        <v>0.97414939548205803</v>
+        <v>0.99910736744806705</v>
       </c>
       <c r="L7">
-        <v>0.58953898430511498</v>
-      </c>
-      <c r="M7">
-        <v>0.587789610464447</v>
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -917,40 +1365,40 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>3.3333333333333299</v>
+      </c>
+      <c r="E8">
+        <v>3.0682327978210602E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>53</v>
+      </c>
+      <c r="H8">
         <v>3</v>
       </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>1.2245616884675899E-2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8">
-        <v>55</v>
-      </c>
-      <c r="H8">
-        <v>16</v>
-      </c>
       <c r="I8">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J8">
-        <v>17.2090909090909</v>
+        <v>63.308176100628899</v>
       </c>
       <c r="K8">
-        <v>0.984270990302614</v>
+        <v>0.99997335890045203</v>
       </c>
       <c r="L8">
-        <v>0.58953898430511498</v>
-      </c>
-      <c r="M8">
-        <v>0.587789610464447</v>
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -958,7 +1406,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -967,31 +1415,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E9">
-        <v>2.1282276238904399E-2</v>
+        <v>3.0682327978210602E-2</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J9">
-        <v>91.781818181818096</v>
+        <v>63.308176100628899</v>
       </c>
       <c r="K9">
-        <v>0.99928950390565097</v>
+        <v>0.99997335890045203</v>
       </c>
       <c r="L9">
-        <v>0.76441394096397397</v>
-      </c>
-      <c r="M9">
-        <v>0.76214565033796799</v>
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -999,7 +1447,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1008,31 +1456,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E10">
-        <v>2.1282276238904399E-2</v>
+        <v>3.0682327978210602E-2</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G10">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J10">
-        <v>91.781818181818096</v>
+        <v>63.308176100628899</v>
       </c>
       <c r="K10">
-        <v>0.99928950390565097</v>
+        <v>0.99997335890045203</v>
       </c>
       <c r="L10">
-        <v>0.76441394096397397</v>
-      </c>
-      <c r="M10">
-        <v>0.76214565033796799</v>
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1040,7 +1488,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1049,31 +1497,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E11">
-        <v>3.1756068764081997E-2</v>
+        <v>4.0703107092234098E-2</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G11">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J11">
-        <v>61.187878787878702</v>
+        <v>47.481132075471699</v>
       </c>
       <c r="K11">
-        <v>0.99998108213721804</v>
+        <v>0.999999205439841</v>
       </c>
       <c r="L11">
-        <v>0.76441394096397397</v>
-      </c>
-      <c r="M11">
-        <v>0.76214565033796799</v>
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1081,7 +1529,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1090,31 +1538,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E12">
-        <v>3.1756068764081997E-2</v>
+        <v>5.0622263670471103E-2</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G12">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J12">
-        <v>61.187878787878702</v>
+        <v>37.984905660377301</v>
       </c>
       <c r="K12">
-        <v>0.99998108213721804</v>
+        <v>0.99999997631919202</v>
       </c>
       <c r="L12">
-        <v>0.76441394096397397</v>
-      </c>
-      <c r="M12">
-        <v>0.76214565033796799</v>
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1122,7 +1570,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1131,31 +1579,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E13">
-        <v>3.1756068764081997E-2</v>
+        <v>7.0159741632765601E-2</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G13">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I13">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J13">
-        <v>61.187878787878702</v>
+        <v>27.132075471698101</v>
       </c>
       <c r="K13">
-        <v>0.99998108213721804</v>
+        <v>0.99999999997900901</v>
       </c>
       <c r="L13">
-        <v>0.76441394096397397</v>
-      </c>
-      <c r="M13">
-        <v>0.76214565033796799</v>
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1163,7 +1611,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1172,31 +1620,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E14">
-        <v>3.1756068764081997E-2</v>
+        <v>7.0159741632765601E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G14">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I14">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J14">
-        <v>61.187878787878702</v>
+        <v>27.132075471698101</v>
       </c>
       <c r="K14">
-        <v>0.99998108213721804</v>
+        <v>0.99999999997900901</v>
       </c>
       <c r="L14">
-        <v>0.76441394096397397</v>
-      </c>
-      <c r="M14">
-        <v>0.76214565033796799</v>
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1204,7 +1652,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1213,31 +1661,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E15">
-        <v>3.1756068764081997E-2</v>
+        <v>7.0159741632765601E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G15">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J15">
-        <v>61.187878787878702</v>
+        <v>27.132075471698101</v>
       </c>
       <c r="K15">
-        <v>0.99998108213721804</v>
+        <v>0.99999999997900901</v>
       </c>
       <c r="L15">
-        <v>0.76441394096397397</v>
-      </c>
-      <c r="M15">
-        <v>0.76214565033796799</v>
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1245,7 +1693,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1254,31 +1702,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E16">
-        <v>5.2374692423957703E-2</v>
+        <v>7.97800546916414E-2</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G16">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I16">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J16">
-        <v>36.7127272727272</v>
+        <v>23.7405660377358</v>
       </c>
       <c r="K16">
-        <v>0.99999998661706802</v>
+        <v>0.99999999999937506</v>
       </c>
       <c r="L16">
         <v>1</v>
       </c>
-      <c r="M16">
-        <v>1</v>
+      <c r="M16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1286,7 +1734,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1295,31 +1743,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E17">
-        <v>7.2562205981846206E-2</v>
+        <v>7.97800546916414E-2</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G17">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I17">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J17">
-        <v>26.223376623376598</v>
+        <v>23.7405660377358</v>
       </c>
       <c r="K17">
-        <v>0.99999999999056</v>
+        <v>0.99999999999937506</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
-      <c r="M17">
-        <v>1</v>
+      <c r="M17" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1327,7 +1775,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1336,31 +1784,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E18">
-        <v>7.2562205981846206E-2</v>
+        <v>7.97800546916414E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="G18">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I18">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J18">
-        <v>26.223376623376598</v>
+        <v>23.7405660377358</v>
       </c>
       <c r="K18">
-        <v>0.99999999999056</v>
+        <v>0.99999999999937506</v>
       </c>
       <c r="L18">
         <v>1</v>
       </c>
-      <c r="M18">
-        <v>1</v>
+      <c r="M18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1368,40 +1816,40 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>8.7425350026652804E-2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19">
+        <v>53</v>
+      </c>
+      <c r="H19">
         <v>48</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>3.3333333333333299</v>
-      </c>
-      <c r="E19">
-        <v>8.2497068285960096E-2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19">
-        <v>55</v>
-      </c>
-      <c r="H19">
-        <v>8</v>
-      </c>
       <c r="I19">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J19">
-        <v>22.945454545454499</v>
+        <v>5.9351415094339597</v>
       </c>
       <c r="K19">
-        <v>0.99999999999974898</v>
+        <v>0.99999999999996203</v>
       </c>
       <c r="L19">
         <v>1</v>
       </c>
-      <c r="M19">
-        <v>1</v>
+      <c r="M19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1409,7 +1857,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1418,31 +1866,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E20">
-        <v>8.2497068285960096E-2</v>
+        <v>9.8728735540591403E-2</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G20">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I20">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J20">
-        <v>22.945454545454499</v>
+        <v>18.992452830188601</v>
       </c>
       <c r="K20">
-        <v>0.99999999999974898</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
-      <c r="M20">
-        <v>1</v>
+      <c r="M20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1450,7 +1898,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1459,31 +1907,31 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E21">
-        <v>8.2497068285960096E-2</v>
+        <v>9.8728735540591403E-2</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="G21">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I21">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J21">
-        <v>22.945454545454499</v>
+        <v>18.992452830188601</v>
       </c>
       <c r="K21">
-        <v>0.99999999999974898</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
-      <c r="M21">
-        <v>1</v>
+      <c r="M21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1491,7 +1939,7 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1500,75 +1948,34 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="E22">
-        <v>9.2327456840091304E-2</v>
+        <v>9.8728735540591403E-2</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G22">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I22">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J22">
-        <v>20.3959595959595</v>
+        <v>18.992452830188601</v>
       </c>
       <c r="K22">
-        <v>0.99999999999999301</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="L22">
         <v>1</v>
       </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-      <c r="E23">
-        <v>9.2770788615935296E-2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23">
-        <v>55</v>
-      </c>
-      <c r="H23">
-        <v>48</v>
-      </c>
-      <c r="I23">
-        <v>5048</v>
-      </c>
-      <c r="J23">
-        <v>5.7363636363636301</v>
-      </c>
-      <c r="K23">
-        <v>0.999999999999994</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
+      <c r="M22" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>